<commit_message>
Month1 objective: app scheleton, logging, observability, workflow endpoint, tests, wire Serilog/OTel, add event log writer, hello workflow, test harness, openapi, scalar, swagger
</commit_message>
<xml_diff>
--- a/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
+++ b/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10125"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippomargiotta/Documents/Personal/AgenticOrchestrationSoftware/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4D1757-ED3E-8044-9649-DAE44E59FEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE6C26A-4EE4-EA4D-AFC2-95A60A4C7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="C12" s="70">
         <f>January!AH14</f>
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D12" s="70">
         <f>February!AE14</f>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="O12" s="69">
         <f>SUM(C12:N12)</f>
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15" customHeight="1">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="C29" s="4">
         <f>SUM(C12:C28)</f>
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" ref="D29:O29" si="1">SUM(D12:D28)</f>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="O29" s="6">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1">
@@ -7739,7 +7739,7 @@
   <dimension ref="A1:AK41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="C3" zoomScale="117" zoomScaleNormal="70" zoomScalePageLayoutView="117" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -7996,7 +7996,9 @@
       <c r="H14" s="17">
         <v>3</v>
       </c>
-      <c r="I14" s="17"/>
+      <c r="I14" s="17">
+        <v>6</v>
+      </c>
       <c r="J14" s="17">
         <v>4</v>
       </c>
@@ -8031,15 +8033,23 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="16"/>
-      <c r="AB14" s="17"/>
-      <c r="AC14" s="17"/>
-      <c r="AD14" s="17"/>
-      <c r="AE14" s="17"/>
+      <c r="AB14" s="17">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="17">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="17">
+        <v>4</v>
+      </c>
+      <c r="AE14" s="17">
+        <v>4</v>
+      </c>
       <c r="AF14" s="17"/>
       <c r="AG14" s="54"/>
       <c r="AH14" s="43">
         <f>SUM(C14:AG14)</f>
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Add local CI script and fix xUnit test discovery
</commit_message>
<xml_diff>
--- a/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
+++ b/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10201"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippomargiotta/Documents/Personal/AgenticOrchestrationSoftware/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippomargiotta/Documents/Personal/AosRepo/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE6C26A-4EE4-EA4D-AFC2-95A60A4C7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129A7F4B-9356-174C-AD2E-C58828F65379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="D12" s="70">
         <f>February!AE14</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E12" s="70">
         <f>March!AH14</f>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="O12" s="69">
         <f>SUM(C12:N12)</f>
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15" customHeight="1">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" ref="D29:O29" si="1">SUM(D12:D28)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="1"/>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="O29" s="6">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1">
@@ -7738,7 +7738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="C3" zoomScale="117" zoomScaleNormal="70" zoomScalePageLayoutView="117" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="C14" zoomScale="117" zoomScaleNormal="70" zoomScalePageLayoutView="117" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -8904,8 +8904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -9144,13 +9144,27 @@
         <f>January!B14</f>
         <v>AI-Driven Agentic Orchestration Software (AOC-WebAPI)</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
+      <c r="C14" s="16">
+        <v>4</v>
+      </c>
+      <c r="D14" s="17">
+        <v>4</v>
+      </c>
+      <c r="E14" s="17">
+        <v>4</v>
+      </c>
+      <c r="F14" s="17">
+        <v>4</v>
+      </c>
+      <c r="G14" s="17">
+        <v>4</v>
+      </c>
+      <c r="H14" s="17">
+        <v>4</v>
+      </c>
+      <c r="I14" s="18">
+        <v>6</v>
+      </c>
       <c r="J14" s="16"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
@@ -9174,7 +9188,7 @@
       <c r="AD14" s="54"/>
       <c r="AE14" s="43">
         <f t="shared" ref="AE14:AE30" si="0">SUM(C14:AC14)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" customHeight="1">
@@ -16848,14 +16862,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e61e294-5db2-4ad2-9356-7488524978e7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9160ec49-0786-419e-aae3-9c9cb8f5a974" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17094,23 +17106,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e61e294-5db2-4ad2-9356-7488524978e7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9160ec49-0786-419e-aae3-9c9cb8f5a974" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1149BA22-2185-4279-8D4D-20B81C2A7999}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23919C5-C77D-4D6C-8993-5ED5B021C1A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a022c38d-a398-45a6-8336-4b22e89f761d"/>
-    <ds:schemaRef ds:uri="52db9a4d-0878-46fa-948e-68042efe192b"/>
-    <ds:schemaRef ds:uri="0e61e294-5db2-4ad2-9356-7488524978e7"/>
-    <ds:schemaRef ds:uri="9160ec49-0786-419e-aae3-9c9cb8f5a974"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17135,9 +17144,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23919C5-C77D-4D6C-8993-5ED5B021C1A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1149BA22-2185-4279-8D4D-20B81C2A7999}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a022c38d-a398-45a6-8336-4b22e89f761d"/>
+    <ds:schemaRef ds:uri="52db9a4d-0878-46fa-948e-68042efe192b"/>
+    <ds:schemaRef ds:uri="0e61e294-5db2-4ad2-9356-7488524978e7"/>
+    <ds:schemaRef ds:uri="9160ec49-0786-419e-aae3-9c9cb8f5a974"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{0eea11ca-d417-4147-80ed-01a58412c458}" enabled="1" method="Standard" siteId="{bc9dc15c-61bc-4f03-b60b-e5b6d8922839}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add structured app logging and timestamped local CI output
</commit_message>
<xml_diff>
--- a/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
+++ b/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10208"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippomargiotta/Documents/Personal/AosRepo/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A550E14-9204-7247-9AB2-FEBB97AEB7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BDAFD1-A397-584F-B03E-2269EF32226B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1368,6 +1368,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1382,15 +1391,6 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1936,53 +1936,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:34" ht="58.5" customHeight="1">
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
       <c r="R2" s="36"/>
       <c r="U2" s="36"/>
       <c r="X2" s="36"/>
     </row>
     <row r="3" spans="1:34" ht="24.75" customHeight="1">
-      <c r="A3" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="A3" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1">
-      <c r="A4" s="90"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
+      <c r="A4" s="93"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="93"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="B6" s="77" t="s">
@@ -1994,15 +1994,15 @@
       <c r="B7" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="89"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="92"/>
       <c r="L7" s="79"/>
       <c r="AH7" s="2"/>
     </row>
@@ -2010,15 +2010,15 @@
       <c r="B8" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="87" t="s">
+      <c r="E8" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="89"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="92"/>
       <c r="L8" s="79"/>
       <c r="AH8" s="2"/>
     </row>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="D12" s="70">
         <f>February!AE14</f>
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E12" s="70">
         <f>March!AH14</f>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="O12" s="69">
         <f>SUM(C12:N12)</f>
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15" customHeight="1">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" ref="D29:O29" si="1">SUM(D12:D28)</f>
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="1"/>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="O29" s="6">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1">
@@ -3208,34 +3208,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -3246,32 +3246,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -4341,34 +4341,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -4379,32 +4379,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -5493,34 +5493,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -5531,32 +5531,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -6621,34 +6621,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -6659,32 +6659,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -7780,34 +7780,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:37" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -7818,32 +7818,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:37" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:37" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -8905,7 +8905,7 @@
   <dimension ref="A1:AE41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -8946,34 +8946,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:31" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -8984,32 +8984,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:31" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:31" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -9166,13 +9166,27 @@
         <v>4</v>
       </c>
       <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="16"/>
+      <c r="K14" s="17">
+        <v>4</v>
+      </c>
+      <c r="L14" s="17">
+        <v>4</v>
+      </c>
+      <c r="M14" s="17">
+        <v>6</v>
+      </c>
+      <c r="N14" s="17">
+        <v>6</v>
+      </c>
+      <c r="O14" s="17">
+        <v>4</v>
+      </c>
+      <c r="P14" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>1</v>
+      </c>
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
@@ -9188,7 +9202,7 @@
       <c r="AD14" s="54"/>
       <c r="AE14" s="43">
         <f t="shared" ref="AE14:AE30" si="0">SUM(C14:AC14)</f>
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" customHeight="1">
@@ -10039,34 +10053,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -10077,32 +10091,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -11190,34 +11204,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -11228,32 +11242,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -12318,34 +12332,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -12356,32 +12370,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -13470,34 +13484,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -13508,32 +13522,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -14597,34 +14611,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -14635,32 +14649,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>
@@ -15752,34 +15766,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="78"/>
-      <c r="C5" s="92" t="str">
+      <c r="C5" s="87" t="str">
         <f>Overview!E7</f>
         <v>Filippo Margiotta | 265126642</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="78"/>
-      <c r="C6" s="92" t="str">
+      <c r="C6" s="87" t="str">
         <f>Overview!E8</f>
         <v>Director / Architect</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="89"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="78"/>
@@ -15790,32 +15804,32 @@
         <v>19</v>
       </c>
       <c r="B8" s="78"/>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="89"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="92">
+      <c r="C9" s="87">
         <v>2026</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
     </row>
     <row r="11" spans="1:34" ht="15" customHeight="1">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
Add replay CLI skeleton with tests and finalize February deliverables
</commit_message>
<xml_diff>
--- a/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
+++ b/project/StellaDev WBSO 2026 - Hours registration -  (ENG).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippomargiotta/Documents/Personal/AosRepo/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BDAFD1-A397-584F-B03E-2269EF32226B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C936EB6-0E68-F747-B10B-C14DC3BDBB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="17620" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -1921,7 +1921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH41"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="D12" s="70">
         <f>February!AE14</f>
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E12" s="70">
         <f>March!AH14</f>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="O12" s="69">
         <f>SUM(C12:N12)</f>
-        <v>115</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15" customHeight="1">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" ref="D29:O29" si="1">SUM(D12:D28)</f>
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="1"/>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="O29" s="6">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1">
@@ -8904,8 +8904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -9187,22 +9187,40 @@
       <c r="Q14" s="16">
         <v>1</v>
       </c>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="18"/>
+      <c r="R14" s="17">
+        <v>6</v>
+      </c>
+      <c r="S14" s="17">
+        <v>6</v>
+      </c>
+      <c r="T14" s="17">
+        <v>4</v>
+      </c>
+      <c r="U14" s="17">
+        <v>2</v>
+      </c>
+      <c r="V14" s="17">
+        <v>4</v>
+      </c>
+      <c r="W14" s="18">
+        <v>4</v>
+      </c>
       <c r="X14" s="16"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17"/>
+      <c r="Y14" s="17">
+        <v>6</v>
+      </c>
+      <c r="Z14" s="17">
+        <v>4</v>
+      </c>
       <c r="AA14" s="17"/>
-      <c r="AB14" s="17"/>
+      <c r="AB14" s="17">
+        <v>8</v>
+      </c>
       <c r="AC14" s="17"/>
       <c r="AD14" s="54"/>
       <c r="AE14" s="43">
         <f t="shared" ref="AE14:AE30" si="0">SUM(C14:AC14)</f>
-        <v>59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15" customHeight="1">
@@ -16876,12 +16894,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e61e294-5db2-4ad2-9356-7488524978e7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9160ec49-0786-419e-aae3-9c9cb8f5a974" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17120,20 +17140,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0e61e294-5db2-4ad2-9356-7488524978e7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9160ec49-0786-419e-aae3-9c9cb8f5a974" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23919C5-C77D-4D6C-8993-5ED5B021C1A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1149BA22-2185-4279-8D4D-20B81C2A7999}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a022c38d-a398-45a6-8336-4b22e89f761d"/>
+    <ds:schemaRef ds:uri="52db9a4d-0878-46fa-948e-68042efe192b"/>
+    <ds:schemaRef ds:uri="0e61e294-5db2-4ad2-9356-7488524978e7"/>
+    <ds:schemaRef ds:uri="9160ec49-0786-419e-aae3-9c9cb8f5a974"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17158,14 +17181,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1149BA22-2185-4279-8D4D-20B81C2A7999}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23919C5-C77D-4D6C-8993-5ED5B021C1A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a022c38d-a398-45a6-8336-4b22e89f761d"/>
-    <ds:schemaRef ds:uri="52db9a4d-0878-46fa-948e-68042efe192b"/>
-    <ds:schemaRef ds:uri="0e61e294-5db2-4ad2-9356-7488524978e7"/>
-    <ds:schemaRef ds:uri="9160ec49-0786-419e-aae3-9c9cb8f5a974"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>